<commit_message>
tuning, deadtime, and HW changes
-updated shunt resistor to 200mOhm which may have been too high.  50mOhm seems like an appropriate sweet spot
-added check for nFAULT being asserted LOW, but it does not distinguish between EN_GATE causing nFAULT to go low, vs true faults, so there is more work to be done
-HW change, but I updated the perf-board based breakout of the ODESC pins so I can start developing the LED driver for the RGB led strips via pwm'd dma transfers to GPIO.
</commit_message>
<xml_diff>
--- a/documentation/AS5048A Mag Pinout and Slipring Harness.xlsx
+++ b/documentation/AS5048A Mag Pinout and Slipring Harness.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Github_Repos\Furuta-Pendulum\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC76D2D-8EBA-45B1-933F-B431022DBD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D4619A-28E0-4BCB-AE19-8D0B244A9EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="4260" windowWidth="24540" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11130" yWindow="4020" windowWidth="24540" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>pads on the left, negative terminal on top:</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>odesc pigtail</t>
+  </si>
+  <si>
+    <t>Signal:</t>
+  </si>
+  <si>
+    <t>Wire Color:</t>
   </si>
 </sst>
 </file>
@@ -165,9 +171,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -176,9 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9422054-55A7-4F92-8E4F-D4C2E1C1B847}">
   <dimension ref="C9:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,14 +668,22 @@
   </cols>
   <sheetData>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
@@ -729,13 +744,13 @@
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
@@ -755,161 +770,155 @@
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="2">
         <v>1</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
       <c r="E35" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E36" t="s">
         <v>18</v>
       </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4" t="s">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
       <c r="E37" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4" t="s">
+      <c r="F38" s="2"/>
+      <c r="G38" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
       <c r="E39" t="s">
         <v>24</v>
       </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E40" t="s">
         <v>25</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40" s="2">
         <v>2</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
       <c r="E41" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
       </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4" t="s">
+      <c r="F42" s="2"/>
+      <c r="G42" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
       <c r="E43" t="s">
         <v>28</v>
       </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E44" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4" t="s">
+      <c r="F44" s="2"/>
+      <c r="G44" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
       <c r="E45" t="s">
         <v>27</v>
       </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="G42:G43"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="C44:C45"/>
@@ -926,6 +935,12 @@
     <mergeCell ref="D42:D43"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="G42:G43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -936,7 +951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C9:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>

</xml_diff>